<commit_message>
commiting string practice classes
</commit_message>
<xml_diff>
--- a/MyProject_Practice/ExcelFiles/testfile.xlsx
+++ b/MyProject_Practice/ExcelFiles/testfile.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15195" windowHeight="5970" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Testcases</t>
   </si>
@@ -79,6 +80,24 @@
   </si>
   <si>
     <t>Firefox,Chrome,IE</t>
+  </si>
+  <si>
+    <t>Thread-Count</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>TestCase No</t>
+  </si>
+  <si>
+    <t>module name</t>
+  </si>
+  <si>
+    <t>Test steps</t>
+  </si>
+  <si>
+    <t>EXPECTED RESULT</t>
   </si>
 </sst>
 </file>
@@ -114,8 +133,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,10 +532,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +543,7 @@
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -530,13 +551,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -614,4 +646,34 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>